<commit_message>
auto fill works, but some bugs (cant set all parameters in one cycle, need to click many times)
</commit_message>
<xml_diff>
--- a/SignalGenerationConfigs/UserSignalConfigs/SignalConfigs.xlsx
+++ b/SignalGenerationConfigs/UserSignalConfigs/SignalConfigs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79137\Pasha\Bachelor Thesis Project\Project\SignalGenerationConfigs\UserSignalConfigs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E6696A-74AE-421A-964B-1EF908C72FF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D02E33F-EF27-480B-833C-9F139397F703}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1080" yWindow="2868" windowWidth="2388" windowHeight="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Start Time</t>
   </si>
   <si>
-    <t>TestConfig</t>
-  </si>
-  <si>
     <t>Config Name</t>
   </si>
   <si>
@@ -61,6 +58,12 @@
   </si>
   <si>
     <t>Points Number</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -389,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -410,39 +413,39 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -474,7 +477,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -502,6 +505,38 @@
       </c>
       <c r="J3">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>150</v>
+      </c>
+      <c r="C4">
+        <v>600</v>
+      </c>
+      <c r="D4">
+        <v>300</v>
+      </c>
+      <c r="E4">
+        <v>300</v>
+      </c>
+      <c r="F4" s="1">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>200</v>
+      </c>
+      <c r="I4">
+        <v>100</v>
+      </c>
+      <c r="J4">
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
naive sending code updated
</commit_message>
<xml_diff>
--- a/SignalGenerationConfigs/UserSignalConfigs/SignalConfigs.xlsx
+++ b/SignalGenerationConfigs/UserSignalConfigs/SignalConfigs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79137\Pasha\Bachelor Thesis Project\Project\SignalGenerationConfigs\UserSignalConfigs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9BC769-EDD0-43BD-AA5F-9BF06CBEF961}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242CC292-5FED-4241-92A7-1A5038210C62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-900" yWindow="1812" windowWidth="2388" windowHeight="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -394,8 +394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -448,16 +448,16 @@
         <v>12</v>
       </c>
       <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
         <v>2</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>15</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
@@ -469,10 +469,10 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="J2">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
WORK sending widgets in UserSignal signal generation window
</commit_message>
<xml_diff>
--- a/SignalGenerationConfigs/UserSignalConfigs/SignalConfigs.xlsx
+++ b/SignalGenerationConfigs/UserSignalConfigs/SignalConfigs.xlsx
@@ -522,32 +522,32 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Test</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D3" t="n">
         <v>3</v>
       </c>
       <c r="E3" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G3" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="J3" t="n">
         <v>3</v>
@@ -556,32 +556,32 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>Test</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D4" t="n">
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F4" t="n">
         <v>0.1</v>
       </c>
       <c r="G4" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="J4" t="n">
         <v>3</v>

</xml_diff>